<commit_message>
New boca and ave taxa
</commit_message>
<xml_diff>
--- a/tabular/genus/ave-refseqs-side-data.xlsx
+++ b/tabular/genus/ave-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNA/Parvovirus-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C67050-5E90-374C-9A5A-F6FBC6B4B9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB67D51-15E7-E34A-86C9-664846CC5F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5360" yWindow="8080" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>virus_name</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>Parvovirinae</t>
+  </si>
+  <si>
+    <t>MG745672</t>
+  </si>
+  <si>
+    <t>FinchAvePV</t>
+  </si>
+  <si>
+    <t>Pileated finch aveparvovirus</t>
+  </si>
+  <si>
+    <t>Coryphospingus pileatus</t>
   </si>
 </sst>
 </file>
@@ -2364,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:M4"/>
+      <selection activeCell="D4" sqref="A1:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2549,6 +2561,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M2">
     <sortCondition ref="I2"/>

</xml_diff>